<commit_message>
added an extra figure
</commit_message>
<xml_diff>
--- a/PowerAndThrustData.xlsx
+++ b/PowerAndThrustData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BHRay" sheetId="1" state="visible" r:id="rId2"/>
@@ -420,7 +420,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -544,11 +544,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="41827155"/>
-        <c:axId val="71434394"/>
+        <c:axId val="93942534"/>
+        <c:axId val="73405901"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41827155"/>
+        <c:axId val="93942534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,12 +576,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71434394"/>
+        <c:crossAx val="73405901"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71434394"/>
+        <c:axId val="73405901"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,7 +618,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41827155"/>
+        <c:crossAx val="93942534"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -666,7 +666,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -792,11 +792,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="246454"/>
-        <c:axId val="232955"/>
+        <c:axId val="60414477"/>
+        <c:axId val="6592776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="246454"/>
+        <c:axId val="60414477"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,12 +824,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232955"/>
+        <c:crossAx val="6592776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="232955"/>
+        <c:axId val="6592776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +866,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246454"/>
+        <c:crossAx val="60414477"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -914,7 +914,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1057,11 +1057,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="4916560"/>
-        <c:axId val="45596140"/>
+        <c:axId val="62525596"/>
+        <c:axId val="54883288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4916560"/>
+        <c:axId val="62525596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,12 +1089,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45596140"/>
+        <c:crossAx val="54883288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45596140"/>
+        <c:axId val="54883288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,7 +1131,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4916560"/>
+        <c:crossAx val="62525596"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1158,7 +1158,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1270,42 +1270,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.9822953918306</c:v>
+                  <c:v>0.606582389900164</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.77355495665088</c:v>
+                  <c:v>1.15470781673517</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.16473372386153</c:v>
+                  <c:v>1.88640851950163</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.19436743905976</c:v>
+                  <c:v>2.81347643635229</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.0306749243708</c:v>
+                  <c:v>3.98738652685747</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.2398352731677</c:v>
+                  <c:v>5.27538959358933</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.8417870712421</c:v>
+                  <c:v>6.37758684380009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.8860627773238</c:v>
+                  <c:v>7.92113520986108</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.8086734945154</c:v>
+                  <c:v>10.3454540893217</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="56872841"/>
-        <c:axId val="95356422"/>
+        <c:axId val="79029233"/>
+        <c:axId val="4751868"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56872841"/>
+        <c:axId val="79029233"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,12 +1333,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95356422"/>
+        <c:crossAx val="4751868"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95356422"/>
+        <c:axId val="4751868"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,7 +1375,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56872841"/>
+        <c:crossAx val="79029233"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1434,9 +1434,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>507960</xdr:colOff>
+      <xdr:colOff>507600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1445,7 +1445,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="976680" y="2492640"/>
-        <a:ext cx="5761800" cy="3231720"/>
+        <a:ext cx="5761440" cy="3231360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1469,9 +1469,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>685080</xdr:colOff>
+      <xdr:colOff>684720</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1480,7 +1480,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2265480" y="3368880"/>
-        <a:ext cx="5751720" cy="3231720"/>
+        <a:ext cx="5751360" cy="3231360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1504,9 +1504,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>372240</xdr:colOff>
+      <xdr:colOff>371880</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1515,7 +1515,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="541440" y="4556520"/>
-        <a:ext cx="5751360" cy="3230640"/>
+        <a:ext cx="5751000" cy="3230280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1539,9 +1539,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>524520</xdr:colOff>
+      <xdr:colOff>524160</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1550,7 +1550,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1832400" y="3154680"/>
-        <a:ext cx="5762160" cy="3231720"/>
+        <a:ext cx="5761800" cy="3231360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1571,10 +1571,10 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection pane="topLeft" activeCell="G31" activeCellId="1" sqref="H2:H10 G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9"/>
@@ -2350,10 +2350,10 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
+      <selection pane="topLeft" activeCell="E40" activeCellId="1" sqref="H2:H10 E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.29"/>
@@ -2567,10 +2567,10 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
+      <selection pane="topLeft" activeCell="E54" activeCellId="1" sqref="H2:H10 E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9"/>
@@ -2902,10 +2902,10 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="1" sqref="H2:H10 H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.29"/>
@@ -3269,10 +3269,10 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="H2:H10 L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.29"/>
@@ -4020,10 +4020,10 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="H2:H10 B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.29"/>
@@ -4183,11 +4183,11 @@
   </sheetPr>
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F49" activeCellId="0" sqref="F49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.29"/>
@@ -4253,8 +4253,8 @@
         <v>5.69942196531791</v>
       </c>
       <c r="H2" s="1" t="n">
-        <f aca="false">G2*D2</f>
-        <v>1.9822953918306</v>
+        <f aca="false">G2*D2*B$2</f>
+        <v>0.606582389900164</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -4276,8 +4276,8 @@
         <v>4.90173410404624</v>
       </c>
       <c r="H3" s="1" t="n">
-        <f aca="false">G3*D3</f>
-        <v>3.77355495665088</v>
+        <f aca="false">G3*D3*B$2</f>
+        <v>1.15470781673517</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -4300,8 +4300,8 @@
         <v>3.90751445086705</v>
       </c>
       <c r="H4" s="1" t="n">
-        <f aca="false">G4*D4</f>
-        <v>6.16473372386153</v>
+        <f aca="false">G4*D4*B$2</f>
+        <v>1.88640851950163</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -4324,8 +4324,8 @@
         <v>4.17341040462427</v>
       </c>
       <c r="H5" s="1" t="n">
-        <f aca="false">G5*D5</f>
-        <v>9.19436743905976</v>
+        <f aca="false">G5*D5*B$2</f>
+        <v>2.81347643635229</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -4348,8 +4348,8 @@
         <v>4.69364161849711</v>
       </c>
       <c r="H6" s="1" t="n">
-        <f aca="false">G6*D6</f>
-        <v>13.0306749243708</v>
+        <f aca="false">G6*D6*B$2</f>
+        <v>3.98738652685747</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -4372,8 +4372,8 @@
         <v>5.36416184971098</v>
       </c>
       <c r="H7" s="1" t="n">
-        <f aca="false">G7*D7</f>
-        <v>17.2398352731677</v>
+        <f aca="false">G7*D7*B$2</f>
+        <v>5.27538959358933</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -4396,8 +4396,8 @@
         <v>6.18497109826589</v>
       </c>
       <c r="H8" s="1" t="n">
-        <f aca="false">G8*D8</f>
-        <v>20.8417870712421</v>
+        <f aca="false">G8*D8*B$2</f>
+        <v>6.37758684380009</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -4420,8 +4420,8 @@
         <v>6.97109826589595</v>
       </c>
       <c r="H9" s="1" t="n">
-        <f aca="false">G9*D9</f>
-        <v>25.8860627773238</v>
+        <f aca="false">G9*D9*B$2</f>
+        <v>7.92113520986108</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -4444,8 +4444,8 @@
         <v>8.49710982658959</v>
       </c>
       <c r="H10" s="1" t="n">
-        <f aca="false">G10*D10</f>
-        <v>33.8086734945154</v>
+        <f aca="false">G10*D10*B$2</f>
+        <v>10.3454540893217</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -4489,10 +4489,10 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="H2:H10 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.29"/>
@@ -4626,11 +4626,11 @@
   </sheetPr>
   <dimension ref="A1:AJ20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="1" sqref="H2:H10 D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.37"/>
   </cols>

</xml_diff>